<commit_message>
Resolvido conflito na planilha PlataformaTE
</commit_message>
<xml_diff>
--- a/PlataformaTE.xlsx
+++ b/PlataformaTE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\Arquivos\Desenvolvimento\AutomacaoTE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F71610-CEC8-4D4D-878A-AC24391014B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A692C217-D242-4D28-9F4D-78DE279104D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="280">
   <si>
     <t>Cliente</t>
   </si>
@@ -811,9 +811,6 @@
     <t>Previsao de entrega: 07/03/24 - verificando status da entrega com a transportadora</t>
   </si>
   <si>
-    <t>João Monlevade</t>
-  </si>
-  <si>
     <t>07/03/2024</t>
   </si>
   <si>
@@ -884,21 +881,6 @@
   </si>
   <si>
     <t>05/03/2024 08:43:37</t>
-  </si>
-  <si>
-    <t>RCM LOCAÇAO DE MAQUINAS LTDA</t>
-  </si>
-  <si>
-    <t>01472377000106</t>
-  </si>
-  <si>
-    <t>EVENTOS EXTERNOS CHUVAS  MANIFESTACOES CORONEL FABRICIANO-MG. [Marcar Entrega]</t>
-  </si>
-  <si>
-    <t>05/03/2024 08:43:38</t>
-  </si>
-  <si>
-    <t>Previsão atualizada da entrega: 12/03/2024</t>
   </si>
 </sst>
 </file>
@@ -1488,11 +1470,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R12"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1574,7 +1556,7 @@
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B2" s="9">
         <v>15097846000169</v>
@@ -1583,7 +1565,7 @@
         <v>138633</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>51</v>
@@ -1592,13 +1574,13 @@
         <v>229</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>230</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J2" s="9">
         <v>3</v>
@@ -1639,16 +1621,16 @@
         <v>53</v>
       </c>
       <c r="F3" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>266</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>267</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>54</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J3" s="9">
         <v>3</v>
@@ -1690,13 +1672,13 @@
         <v>229</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>230</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J4" s="9">
         <v>3</v>
@@ -1740,13 +1722,13 @@
         <v>229</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>230</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J5" s="9">
         <v>3</v>
@@ -1772,7 +1754,7 @@
     </row>
     <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B6" s="9">
         <v>27143718000193</v>
@@ -1781,7 +1763,7 @@
         <v>138646</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>53</v>
@@ -1790,13 +1772,13 @@
         <v>35</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>42</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J6" s="9">
         <v>3</v>
@@ -1814,22 +1796,22 @@
         <v>138646</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="P6" s="8"/>
     </row>
     <row r="7" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>273</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>274</v>
       </c>
       <c r="C7" s="9">
         <v>138647</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>33</v>
@@ -1838,13 +1820,13 @@
         <v>226</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>30</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J7" s="9">
         <v>3</v>
@@ -1862,7 +1844,7 @@
         <v>138647</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="P7" s="8"/>
     </row>
@@ -1886,13 +1868,13 @@
         <v>229</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>230</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J8" s="9">
         <v>3</v>
@@ -1936,13 +1918,13 @@
         <v>229</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>230</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J9" s="9">
         <v>3</v>
@@ -1968,16 +1950,16 @@
     </row>
     <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>277</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>278</v>
       </c>
       <c r="C10" s="9">
         <v>138671</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>33</v>
@@ -1986,13 +1968,13 @@
         <v>226</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>30</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J10" s="9">
         <v>3</v>
@@ -2036,13 +2018,13 @@
         <v>229</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>230</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J11" s="9">
         <v>3</v>
@@ -2065,61 +2047,13 @@
       <c r="P11" s="10">
         <v>45358</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="C12" s="9">
-        <v>138679</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="J12" s="9">
-        <v>3</v>
-      </c>
-      <c r="K12" s="9">
-        <v>2</v>
-      </c>
-      <c r="L12" s="9">
-        <v>8</v>
-      </c>
-      <c r="M12" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="N12" s="9">
-        <v>138679</v>
-      </c>
-      <c r="O12" s="11" t="s">
-        <v>285</v>
-      </c>
-      <c r="P12" s="8"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:R1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <customSheetViews>
     <customSheetView guid="{F4E47935-89ED-4945-9CD3-947E4497D6BA}" filter="1" showAutoFilter="1">
       <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-      <autoFilter ref="B1:P984" xr:uid="{569C5953-B082-4C84-825D-8ABBD1EB1B01}"/>
+      <autoFilter ref="B1:P984" xr:uid="{043C2290-6741-48D3-91C1-4341C738D741}"/>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">
           <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="810247410"/>
@@ -2144,18 +2078,18 @@
     <cfRule type="duplicateValues" dxfId="8" priority="590"/>
     <cfRule type="duplicateValues" dxfId="7" priority="591"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13:C1048576 C1">
+  <conditionalFormatting sqref="C12:C1048576 C1">
     <cfRule type="duplicateValues" dxfId="6" priority="592"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1">
     <cfRule type="duplicateValues" dxfId="5" priority="334"/>
     <cfRule type="duplicateValues" dxfId="4" priority="345"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C12">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+  <conditionalFormatting sqref="C2:C11">
+    <cfRule type="duplicateValues" dxfId="1" priority="593"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C10:C12">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  <conditionalFormatting sqref="C10:C11">
+    <cfRule type="duplicateValues" dxfId="0" priority="594"/>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -4367,10 +4301,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C7">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
removendo nova coluna na analise da planilha
</commit_message>
<xml_diff>
--- a/PlataformaTE.xlsx
+++ b/PlataformaTE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\Arquivos\Desenvolvimento\AutomacaoTE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C762E6A3-BA4F-4262-B11C-E76C29B0FCDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2726C6C0-8515-4E89-9AAF-B97F7D8F3145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,8 +17,8 @@
     <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$R$1</definedName>
-    <definedName name="Z_F4E47935_89ED_4945_9CD3_947E4497D6BA_.wvu.FilterData" localSheetId="0" hidden="1">Sheet1!$B$1:$P$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$S$14</definedName>
+    <definedName name="Z_F4E47935_89ED_4945_9CD3_947E4497D6BA_.wvu.FilterData" localSheetId="0" hidden="1">Sheet1!$B$1:$Q$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="303">
   <si>
     <t>Cliente</t>
   </si>
@@ -808,85 +808,157 @@
     <t>Bauru</t>
   </si>
   <si>
-    <t>Previsao de entrega: 07/03/24 - verificando status da entrega com a transportadora</t>
-  </si>
-  <si>
-    <t>07/03/2024</t>
-  </si>
-  <si>
-    <t>08/03/2024 07:07:07</t>
-  </si>
-  <si>
-    <t>05/03/2024 08:43:32</t>
-  </si>
-  <si>
-    <t>06/03/2024 06:21:00</t>
-  </si>
-  <si>
-    <t>05/03/2024 08:43:34</t>
-  </si>
-  <si>
-    <t>J. L. LIMA TRANSPORTES LTDA</t>
-  </si>
-  <si>
-    <t>SIQUEIRA CAMPOS</t>
-  </si>
-  <si>
-    <t>07/03/2024 06:35:00</t>
-  </si>
-  <si>
-    <t>05/03/2024 08:43:33</t>
-  </si>
-  <si>
-    <t>SP3077232E [Marcar Entrega]</t>
-  </si>
-  <si>
-    <t>03/05/2024 21:20:47</t>
-  </si>
-  <si>
-    <t>05/03/2024 08:43:36</t>
-  </si>
-  <si>
-    <t>05/03/2024 08:43:35</t>
-  </si>
-  <si>
-    <t>VIACAO MARILANDIA LTDA</t>
-  </si>
-  <si>
-    <t>COLATINA</t>
-  </si>
-  <si>
-    <t>Previsao de entrega: 08/03/24.</t>
-  </si>
-  <si>
-    <t>TUCANO S TERRAPLENAGENS E CONSTRUCOES LT</t>
-  </si>
-  <si>
-    <t>03040646000190</t>
-  </si>
-  <si>
-    <t>Presidente Prudente</t>
-  </si>
-  <si>
-    <t>Previsão atualizada da entrega: 08/03/2024</t>
-  </si>
-  <si>
-    <t>VALE DA MADEIRA COMERCIO E LOGISTICA DE</t>
-  </si>
-  <si>
-    <t>05072741000100</t>
-  </si>
-  <si>
-    <t>GARCA</t>
-  </si>
-  <si>
-    <t>05/03/2024 08:43:37</t>
+    <t>NA ORIGEM [Marcar Entrega]</t>
+  </si>
+  <si>
+    <t>13/03/2024</t>
+  </si>
+  <si>
+    <t>15/03/2024 06:56:26</t>
+  </si>
+  <si>
+    <t>CAM SYSTEM DO BRASIL COMERCIO DE EQUIPAM</t>
+  </si>
+  <si>
+    <t>03946079000136</t>
+  </si>
+  <si>
+    <t>Valinhos</t>
+  </si>
+  <si>
+    <t>MENEGAS TERRAPL. DEMOLICAO E INFRA. LTDA</t>
+  </si>
+  <si>
+    <t>07461125000168</t>
+  </si>
+  <si>
+    <t>RIBEIRAO PRETO</t>
+  </si>
+  <si>
+    <t>13/03/2024 08:48:41</t>
+  </si>
+  <si>
+    <t>VANDERLEI DA SILVA TURTERA</t>
+  </si>
+  <si>
+    <t>GUARUJA</t>
+  </si>
+  <si>
+    <t>EM TRÂNSITO PARA A UNIDADE DE TRANSFERÊNCIA DE SAO PAULO-SP, COM PREVISÃO DE CHEGADA EM 14/03/2024 00:36. [Marcar Entrega]</t>
+  </si>
+  <si>
+    <t>13/03/2024 08:48:42</t>
+  </si>
+  <si>
+    <t>Vendedor</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Previsao de entrega 18/03</t>
+  </si>
+  <si>
+    <t>14/03/2024</t>
+  </si>
+  <si>
+    <t>15/03/2024 07:59:00</t>
+  </si>
+  <si>
+    <t>TRATOL TRATORES PECAS E SERVICOS LT DA -</t>
+  </si>
+  <si>
+    <t>01671306000132</t>
+  </si>
+  <si>
+    <t>17/03/2024 21:51:32</t>
+  </si>
+  <si>
+    <t>13/03/2024 08:48:40</t>
+  </si>
+  <si>
+    <t>Previsão de entrega: 20/03/2024</t>
+  </si>
+  <si>
+    <t>13/03/2024 08:48:37</t>
+  </si>
+  <si>
+    <t>RCM LOCAÇAO DE MAQUINAS LTDA</t>
+  </si>
+  <si>
+    <t>01472377000106</t>
+  </si>
+  <si>
+    <t>João Monlevade</t>
+  </si>
+  <si>
+    <t>DANIELSOARES (161)</t>
+  </si>
+  <si>
+    <t>EM TRÂNSITO PARA A UNIDADE DE TRANSFERÊNCIA DE CONTAGEM-MG, COM PREVISÃO DE CHEGADA EM 14/03/2024 14:08. [Marcar Entrega]</t>
+  </si>
+  <si>
+    <t>13/03/2024 08:48:43</t>
+  </si>
+  <si>
+    <t>WEBCONTINENTAL LTDA</t>
+  </si>
+  <si>
+    <t>08584116000470</t>
+  </si>
+  <si>
+    <t>VIANA</t>
+  </si>
+  <si>
+    <t>GEANDIAS (24)</t>
+  </si>
+  <si>
+    <t>13/03/2024 08:48:45</t>
+  </si>
+  <si>
+    <t>14/03/2024 08:25:45</t>
+  </si>
+  <si>
+    <t>GISELI DE FATIMA DA SILVA GONCALVES &amp; CI</t>
+  </si>
+  <si>
+    <t>Santa Rita do Sapucaí</t>
+  </si>
+  <si>
+    <t>EM TRÂNSITO PARA A UNIDADE DE DISTRIBUIÇÃO DE ALFENAS-MG, COM PREVISÃO DE CHEGADA EM 15/03/2024 07:07. [Marcar Entrega]</t>
+  </si>
+  <si>
+    <t>Previsão de entrega: 18/03/2024</t>
+  </si>
+  <si>
+    <t>14/03/2024 08:25:48</t>
+  </si>
+  <si>
+    <t>TIAGO FRANCISCO DE SOUZA 09268040654</t>
+  </si>
+  <si>
+    <t>SAO SEBASTIAO DO PARAISO</t>
+  </si>
+  <si>
+    <t>MERCADORIA DISPONÍVEL PARA SER RETIRADA. [Marcar Entrega]</t>
+  </si>
+  <si>
+    <t>Previsão atualizada da entrega: 08/04/2024, verificando com a transportadora Previsão de entrega: 20/03/2024</t>
+  </si>
+  <si>
+    <t>EM ENTREGA [Marcar Entrega]</t>
+  </si>
+  <si>
+    <t>14/03/2024 08:25:52</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0;\(#,##0\)"/>
+  </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -946,7 +1018,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -963,6 +1035,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1002,7 +1080,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1023,125 +1101,17 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{5FA7E8DA-F6F0-4F04-83F8-2C6B95C1A608}"/>
     <cellStyle name="Normal 3" xfId="2" xr:uid="{C5C270AF-2E3A-4FBD-9257-6BC41C9504C2}"/>
   </cellStyles>
-  <dxfs count="22">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="11">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1463,11 +1433,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1477,21 +1447,22 @@
     <col min="3" max="3" width="8.42578125" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="6" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" customWidth="1"/>
-    <col min="10" max="10" width="5.5703125" customWidth="1"/>
-    <col min="11" max="12" width="8.140625" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" customWidth="1"/>
-    <col min="15" max="15" width="30.140625" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" customWidth="1"/>
-    <col min="17" max="17" width="17.5703125" customWidth="1"/>
-    <col min="18" max="18" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" customWidth="1"/>
+    <col min="11" max="11" width="5.5703125" customWidth="1"/>
+    <col min="12" max="13" width="8.140625" customWidth="1"/>
+    <col min="14" max="14" width="9.42578125" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" customWidth="1"/>
+    <col min="16" max="16" width="30.140625" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" customWidth="1"/>
+    <col min="18" max="18" width="17.5703125" customWidth="1"/>
+    <col min="19" max="19" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1508,340 +1479,363 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>274</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="C2" s="9">
+        <v>139025</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="17">
+        <v>0</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="K2" s="9">
+        <v>4</v>
+      </c>
+      <c r="L2" s="9">
+        <v>2</v>
+      </c>
+      <c r="M2" s="9">
+        <v>8</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="O2" s="9">
+        <v>139025</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q2" s="10"/>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="B3" s="9">
+        <v>26627354000235</v>
+      </c>
+      <c r="C3" s="9">
+        <v>139027</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="17">
+        <v>0</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="K3" s="9">
+        <v>4</v>
+      </c>
+      <c r="L3" s="9">
+        <v>5</v>
+      </c>
+      <c r="M3" s="9">
+        <v>13</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="9">
+        <v>139027</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q3" s="10">
+        <v>45366</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="C4" s="9">
+        <v>139031</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="K4" s="9">
+        <v>4</v>
+      </c>
+      <c r="L4" s="9">
+        <v>2</v>
+      </c>
+      <c r="M4" s="9">
+        <v>8</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="O4" s="9">
+        <v>139031</v>
+      </c>
+      <c r="P4" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q4" s="10"/>
+    </row>
+    <row r="5" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>261</v>
       </c>
-      <c r="B2" s="9">
-        <v>15097846000169</v>
-      </c>
-      <c r="C2" s="9">
-        <v>138633</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="B5" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="G2" s="8" t="s">
+      <c r="C5" s="9">
+        <v>139039</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="I2" s="8" t="s">
+      <c r="E5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="8" t="s">
         <v>264</v>
       </c>
-      <c r="J2" s="9">
-        <v>3</v>
-      </c>
-      <c r="K2" s="9">
-        <v>5</v>
-      </c>
-      <c r="L2" s="9">
-        <v>13</v>
-      </c>
-      <c r="M2" s="8" t="s">
+      <c r="K5" s="9">
+        <v>2</v>
+      </c>
+      <c r="L5" s="9">
+        <v>1</v>
+      </c>
+      <c r="M5" s="9">
+        <v>7</v>
+      </c>
+      <c r="N5" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="N2" s="9">
-        <v>138633</v>
-      </c>
-      <c r="O2" s="8" t="s">
+      <c r="O5" s="9">
+        <v>139039</v>
+      </c>
+      <c r="P5" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="P2" s="10">
-        <v>45358</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="B3" s="9">
-        <v>29146234000123</v>
-      </c>
-      <c r="C3" s="9">
-        <v>138635</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="8" t="s">
+      <c r="Q5" s="10">
+        <v>45366</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="B6" s="9">
+        <v>10142962000139</v>
+      </c>
+      <c r="C6" s="9">
+        <v>139047</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>266</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="I3" s="8" t="s">
+      <c r="E6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>267</v>
       </c>
-      <c r="J3" s="9">
-        <v>3</v>
-      </c>
-      <c r="K3" s="9">
-        <v>2</v>
-      </c>
-      <c r="L3" s="9">
-        <v>8</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="N3" s="15">
-        <v>138635</v>
-      </c>
-      <c r="O3" s="14" t="s">
-        <v>255</v>
-      </c>
-      <c r="P3" s="10"/>
-    </row>
-    <row r="4" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="B4" s="9">
-        <v>26627354000235</v>
-      </c>
-      <c r="C4" s="9">
-        <v>138642</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="J4" s="9">
-        <v>3</v>
-      </c>
-      <c r="K4" s="9">
-        <v>5</v>
-      </c>
-      <c r="L4" s="9">
-        <v>13</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="N4" s="9">
-        <v>138642</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="P4" s="10">
-        <v>45358</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="B5" s="9">
-        <v>26627354000235</v>
-      </c>
-      <c r="C5" s="9">
-        <v>138645</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="J5" s="9">
-        <v>3</v>
-      </c>
-      <c r="K5" s="9">
-        <v>5</v>
-      </c>
-      <c r="L5" s="9">
-        <v>13</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="N5" s="9">
-        <v>138645</v>
-      </c>
-      <c r="O5" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="P5" s="10">
-        <v>45358</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="B6" s="9">
-        <v>27143718000193</v>
-      </c>
-      <c r="C6" s="9">
-        <v>138646</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>256</v>
-      </c>
       <c r="H6" s="8" t="s">
-        <v>42</v>
+        <v>257</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="J6" s="9">
-        <v>3</v>
+        <v>30</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>264</v>
       </c>
       <c r="K6" s="9">
         <v>2</v>
       </c>
       <c r="L6" s="9">
-        <v>8</v>
-      </c>
-      <c r="M6" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="M6" s="9">
+        <v>7</v>
+      </c>
+      <c r="N6" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="N6" s="9">
-        <v>138646</v>
-      </c>
-      <c r="O6" s="11" t="s">
-        <v>271</v>
-      </c>
-      <c r="P6" s="8"/>
-    </row>
-    <row r="7" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O6" s="9">
+        <v>139047</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q6" s="10">
+        <v>45366</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>272</v>
-      </c>
-      <c r="B7" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="B7" s="9">
+        <v>26627354000235</v>
+      </c>
+      <c r="C7" s="9">
+        <v>139049</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="17">
+        <v>0</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="H7" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="C7" s="9">
-        <v>138647</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>274</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>257</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>30</v>
-      </c>
       <c r="I7" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="J7" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="J7" s="9">
-        <v>3</v>
-      </c>
       <c r="K7" s="9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L7" s="9">
-        <v>7</v>
-      </c>
-      <c r="M7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="M7" s="9">
+        <v>13</v>
+      </c>
+      <c r="N7" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="N7" s="9">
-        <v>138647</v>
-      </c>
-      <c r="O7" s="11" t="s">
-        <v>275</v>
-      </c>
-      <c r="P7" s="8"/>
-    </row>
-    <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O7" s="9">
+        <v>139049</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q7" s="10">
+        <v>45366</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>231</v>
       </c>
@@ -1849,7 +1843,7 @@
         <v>26627354000235</v>
       </c>
       <c r="C8" s="9">
-        <v>138656</v>
+        <v>139066</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>228</v>
@@ -1857,196 +1851,361 @@
       <c r="E8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="17">
+        <v>0</v>
+      </c>
+      <c r="G8" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="H8" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="K8" s="9">
+        <v>4</v>
+      </c>
+      <c r="L8" s="9">
+        <v>5</v>
+      </c>
+      <c r="M8" s="9">
+        <v>13</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="O8" s="9">
+        <v>139066</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q8" s="10">
+        <v>45366</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="C9" s="9">
+        <v>139083</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="K9" s="9">
+        <v>4</v>
+      </c>
+      <c r="L9" s="9">
+        <v>2</v>
+      </c>
+      <c r="M9" s="9">
+        <v>8</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="O9" s="9">
+        <v>139083</v>
+      </c>
+      <c r="P9" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="Q9" s="10"/>
+    </row>
+    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="B10" s="9">
+        <v>26627354000235</v>
+      </c>
+      <c r="C10" s="9">
+        <v>139099</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="17">
+        <v>0</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="K10" s="9">
+        <v>3</v>
+      </c>
+      <c r="L10" s="9">
+        <v>5</v>
+      </c>
+      <c r="M10" s="9">
+        <v>13</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="O10" s="9">
+        <v>139099</v>
+      </c>
+      <c r="P10" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q10" s="10">
+        <v>45366</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="B11" s="9">
+        <v>19751137000106</v>
+      </c>
+      <c r="C11" s="9">
+        <v>139102</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="K11" s="9">
+        <v>3</v>
+      </c>
+      <c r="L11" s="9">
+        <v>2</v>
+      </c>
+      <c r="M11" s="9">
+        <v>8</v>
+      </c>
+      <c r="N11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="O11" s="9">
+        <v>139102</v>
+      </c>
+      <c r="P11" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="Q11" s="10"/>
+    </row>
+    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="B12" s="9">
+        <v>26627354000235</v>
+      </c>
+      <c r="C12" s="9">
+        <v>139115</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="17">
+        <v>0</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="K12" s="9">
+        <v>3</v>
+      </c>
+      <c r="L12" s="9">
+        <v>5</v>
+      </c>
+      <c r="M12" s="9">
+        <v>13</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="O12" s="9">
+        <v>139115</v>
+      </c>
+      <c r="P12" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q12" s="10">
+        <v>45366</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="B13" s="9">
+        <v>36709883000150</v>
+      </c>
+      <c r="C13" s="9">
+        <v>139116</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="K13" s="9">
+        <v>3</v>
+      </c>
+      <c r="L13" s="9">
+        <v>2</v>
+      </c>
+      <c r="M13" s="9">
+        <v>8</v>
+      </c>
+      <c r="N13" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="O13" s="15">
+        <v>139116</v>
+      </c>
+      <c r="P13" s="16" t="s">
+        <v>300</v>
+      </c>
+      <c r="Q13" s="10"/>
+    </row>
+    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="H8" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>267</v>
-      </c>
-      <c r="J8" s="9">
+      <c r="C14" s="9">
+        <v>139133</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="17">
+        <v>0</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="K14" s="9">
         <v>3</v>
       </c>
-      <c r="K8" s="9">
-        <v>5</v>
-      </c>
-      <c r="L8" s="9">
-        <v>13</v>
-      </c>
-      <c r="M8" s="8" t="s">
+      <c r="L14" s="9">
+        <v>1</v>
+      </c>
+      <c r="M14" s="9">
+        <v>7</v>
+      </c>
+      <c r="N14" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="N8" s="9">
-        <v>138656</v>
-      </c>
-      <c r="O8" s="8" t="s">
+      <c r="O14" s="9">
+        <v>139133</v>
+      </c>
+      <c r="P14" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="P8" s="10">
-        <v>45358</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="B9" s="9">
-        <v>26627354000235</v>
-      </c>
-      <c r="C9" s="9">
-        <v>138666</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>260</v>
-      </c>
-      <c r="J9" s="9">
-        <v>3</v>
-      </c>
-      <c r="K9" s="9">
-        <v>5</v>
-      </c>
-      <c r="L9" s="9">
-        <v>13</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="N9" s="9">
-        <v>138666</v>
-      </c>
-      <c r="O9" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="P9" s="10">
-        <v>45358</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>277</v>
-      </c>
-      <c r="C10" s="9">
-        <v>138671</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>257</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="J10" s="9">
-        <v>3</v>
-      </c>
-      <c r="K10" s="9">
-        <v>1</v>
-      </c>
-      <c r="L10" s="9">
-        <v>7</v>
-      </c>
-      <c r="M10" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="N10" s="9">
-        <v>138671</v>
-      </c>
-      <c r="O10" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="P10" s="10">
-        <v>45358</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="B11" s="9">
-        <v>26627354000235</v>
-      </c>
-      <c r="C11" s="9">
-        <v>138674</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="J11" s="9">
-        <v>3</v>
-      </c>
-      <c r="K11" s="9">
-        <v>5</v>
-      </c>
-      <c r="L11" s="9">
-        <v>13</v>
-      </c>
-      <c r="M11" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="N11" s="9">
-        <v>138674</v>
-      </c>
-      <c r="O11" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="P11" s="10">
-        <v>45358</v>
+      <c r="Q14" s="10">
+        <v>45366</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:S14" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <customSheetViews>
     <customSheetView guid="{F4E47935-89ED-4945-9CD3-947E4497D6BA}" filter="1" showAutoFilter="1">
       <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-      <autoFilter ref="B1:P984" xr:uid="{043C2290-6741-48D3-91C1-4341C738D741}"/>
+      <autoFilter ref="B1:P984" xr:uid="{5CF7C203-3BA1-4131-8F9A-1E81233888F0}"/>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">
           <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="810247410"/>
@@ -2054,35 +2213,18 @@
       </extLst>
     </customSheetView>
   </customSheetViews>
-  <conditionalFormatting sqref="C1">
-    <cfRule type="duplicateValues" dxfId="21" priority="395"/>
-    <cfRule type="duplicateValues" dxfId="20" priority="396"/>
-    <cfRule type="duplicateValues" dxfId="19" priority="397"/>
-    <cfRule type="duplicateValues" dxfId="18" priority="398"/>
-    <cfRule type="duplicateValues" dxfId="17" priority="458"/>
-    <cfRule type="duplicateValues" dxfId="16" priority="459"/>
-    <cfRule type="duplicateValues" dxfId="15" priority="460"/>
-    <cfRule type="duplicateValues" dxfId="14" priority="461"/>
-    <cfRule type="duplicateValues" dxfId="13" priority="509"/>
-    <cfRule type="duplicateValues" dxfId="12" priority="581"/>
-    <cfRule type="duplicateValues" dxfId="11" priority="582"/>
-    <cfRule type="duplicateValues" dxfId="10" priority="583"/>
-    <cfRule type="duplicateValues" dxfId="9" priority="589"/>
-    <cfRule type="duplicateValues" dxfId="8" priority="590"/>
-    <cfRule type="duplicateValues" dxfId="7" priority="591"/>
+  <conditionalFormatting sqref="O1">
+    <cfRule type="duplicateValues" dxfId="6" priority="390"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="401"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C12:C1048576 C1">
-    <cfRule type="duplicateValues" dxfId="6" priority="592"/>
+  <conditionalFormatting sqref="C1 C15:C1048576">
+    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1">
-    <cfRule type="duplicateValues" dxfId="5" priority="334"/>
-    <cfRule type="duplicateValues" dxfId="4" priority="345"/>
+  <conditionalFormatting sqref="C2:C14">
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C11">
-    <cfRule type="duplicateValues" dxfId="1" priority="593"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C10:C11">
-    <cfRule type="duplicateValues" dxfId="0" priority="594"/>
+  <conditionalFormatting sqref="C2:C14">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -4294,10 +4436,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C7">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
clean cod, less comments
</commit_message>
<xml_diff>
--- a/PlataformaTE.xlsx
+++ b/PlataformaTE.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\Arquivos\Desenvolvimento\AutomacaoTE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0C1CA6-11E2-4227-940E-849FC0E378C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F91FFC42-0686-4C62-8B18-4C8B1EAFCF7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$S$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$S$1</definedName>
     <definedName name="Z_F4E47935_89ED_4945_9CD3_947E4497D6BA_.wvu.FilterData" localSheetId="0" hidden="1">Sheet1!$B$1:$Q$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="260">
   <si>
     <t>Cliente</t>
   </si>
@@ -811,19 +811,16 @@
     <t>Vendedor</t>
   </si>
   <si>
-    <t>UNIAO COMERCIAL BARAO S/A LOCACAO E EMPR</t>
-  </si>
-  <si>
-    <t>Parauapebas</t>
-  </si>
-  <si>
-    <t>14/03/2024 06:15:58</t>
-  </si>
-  <si>
-    <t>13/03/2024 08:48:44</t>
-  </si>
-  <si>
-    <t>Previsão de entrega atualizada até 19/03 ç</t>
+    <t>26/06/2024 10:10:56</t>
+  </si>
+  <si>
+    <t>24/06/2024 10:30:04</t>
+  </si>
+  <si>
+    <t>24/06/2024 10:30:07</t>
+  </si>
+  <si>
+    <t>24/06/2024 10:30:06</t>
   </si>
 </sst>
 </file>
@@ -942,12 +939,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -968,26 +966,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{5FA7E8DA-F6F0-4F04-83F8-2C6B95C1A608}"/>
     <cellStyle name="Normal 3" xfId="2" xr:uid="{C5C270AF-2E3A-4FBD-9257-6BC41C9504C2}"/>
+    <cellStyle name="Normal 4" xfId="3" xr:uid="{2E9F3EA7-376B-4551-84C1-D324B6977A79}"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1249,11 +1239,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1338,38 +1328,38 @@
       </c>
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="B2" s="9">
+        <v>26627354000235</v>
+      </c>
+      <c r="C2" s="9">
+        <v>144098</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="16">
+        <v>0</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="B2" s="9">
-        <v>57751205851</v>
-      </c>
-      <c r="C2" s="9">
-        <v>138727</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="I2" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2" s="15">
-        <v>0</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="K2" s="9">
-        <v>5</v>
+      <c r="K2" s="15">
+        <v>2</v>
       </c>
       <c r="L2" s="9">
         <v>5</v>
@@ -1377,23 +1367,131 @@
       <c r="M2" s="9">
         <v>13</v>
       </c>
-      <c r="N2" s="8" t="s">
-        <v>38</v>
+      <c r="N2" s="14" t="s">
+        <v>58</v>
       </c>
       <c r="O2" s="9">
-        <v>139070</v>
-      </c>
-      <c r="P2" s="16" t="s">
-        <v>260</v>
-      </c>
-      <c r="Q2" s="10"/>
+        <v>144098</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q2" s="10">
+        <v>45469</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="B3" s="9">
+        <v>26627354000235</v>
+      </c>
+      <c r="C3" s="9">
+        <v>144112</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="16">
+        <v>0</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="K3" s="15">
+        <v>2</v>
+      </c>
+      <c r="L3" s="9">
+        <v>5</v>
+      </c>
+      <c r="M3" s="9">
+        <v>13</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="O3" s="9">
+        <v>144112</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q3" s="10">
+        <v>45469</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="B4" s="9">
+        <v>26627354000235</v>
+      </c>
+      <c r="C4" s="9">
+        <v>144114</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="16">
+        <v>0</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="K4" s="15">
+        <v>2</v>
+      </c>
+      <c r="L4" s="9">
+        <v>5</v>
+      </c>
+      <c r="M4" s="9">
+        <v>13</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="O4" s="9">
+        <v>144114</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q4" s="10">
+        <v>45469</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:S2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:S1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <customSheetViews>
     <customSheetView guid="{F4E47935-89ED-4945-9CD3-947E4497D6BA}" filter="1" showAutoFilter="1">
       <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-      <autoFilter ref="B1:P984" xr:uid="{D93817C6-DA38-4E24-B918-FD68CA12C3BE}"/>
+      <autoFilter ref="B1:P984" xr:uid="{B9A17C03-EB25-4BE9-A236-F0EEFCF55D1B}"/>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">
           <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="810247410"/>
@@ -1401,15 +1499,12 @@
       </extLst>
     </customSheetView>
   </customSheetViews>
-  <conditionalFormatting sqref="C3:C1048576 C1">
-    <cfRule type="duplicateValues" dxfId="5" priority="17"/>
+  <conditionalFormatting sqref="O1">
+    <cfRule type="duplicateValues" dxfId="4" priority="714"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="725"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1">
-    <cfRule type="duplicateValues" dxfId="4" priority="404"/>
-    <cfRule type="duplicateValues" dxfId="3" priority="415"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2">
-    <cfRule type="duplicateValues" dxfId="0" priority="416"/>
+  <conditionalFormatting sqref="C2:C4">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -1421,7 +1516,7 @@
   <dimension ref="A1:P52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:P7"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3621,10 +3716,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C7">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
import time just file pegar_posicao.py
</commit_message>
<xml_diff>
--- a/PlataformaTE.xlsx
+++ b/PlataformaTE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\Arquivos\Desenvolvimento\AutomacaoTE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F91FFC42-0686-4C62-8B18-4C8B1EAFCF7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1250525D-486A-45B5-9991-32A0FC3CA68A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="368">
   <si>
     <t>Cliente</t>
   </si>
@@ -814,13 +814,337 @@
     <t>26/06/2024 10:10:56</t>
   </si>
   <si>
-    <t>24/06/2024 10:30:04</t>
-  </si>
-  <si>
-    <t>24/06/2024 10:30:07</t>
-  </si>
-  <si>
-    <t>24/06/2024 10:30:06</t>
+    <t>MATEUSNATANAEL (172)</t>
+  </si>
+  <si>
+    <t>RENANARAUJO (181)</t>
+  </si>
+  <si>
+    <t>CHEGADA EM UNIDADE (83) [Marcar Entrega]</t>
+  </si>
+  <si>
+    <t>TW Transporte</t>
+  </si>
+  <si>
+    <t>RICARDO SILVA (116)</t>
+  </si>
+  <si>
+    <t>LUCASFARIA (28)</t>
+  </si>
+  <si>
+    <t>SOMA LOGISTICA E LOCACOES LTDA</t>
+  </si>
+  <si>
+    <t>05476099000388</t>
+  </si>
+  <si>
+    <t>NA ORIGEM [Marcar Entrega]</t>
+  </si>
+  <si>
+    <t>17/06/2024</t>
+  </si>
+  <si>
+    <t>14/06/2024 16:34:45</t>
+  </si>
+  <si>
+    <t>destinatario mudou de endereco, novo endereco repassado para Braspress</t>
+  </si>
+  <si>
+    <t>FAZENDA DOIS RIOS LTDA.</t>
+  </si>
+  <si>
+    <t>07057887000284</t>
+  </si>
+  <si>
+    <t>LAGOA DA CONFUSAO</t>
+  </si>
+  <si>
+    <t>ENTRADA NO DEPOSITO [Marcar Entrega]</t>
+  </si>
+  <si>
+    <t>20/06/2024 20:18:43</t>
+  </si>
+  <si>
+    <t>14/06/2024 16:34:53</t>
+  </si>
+  <si>
+    <t>Veiculo retido no posto fiscal - Prev. Atualizada 02/07, solicitando prioridade</t>
+  </si>
+  <si>
+    <t>JG TERRAPLANAGEM</t>
+  </si>
+  <si>
+    <t>Novo Oriente de Minas</t>
+  </si>
+  <si>
+    <t>25/06/2024</t>
+  </si>
+  <si>
+    <t>18/06/2024 08:18:19</t>
+  </si>
+  <si>
+    <t>Previsao de entrega: 02/07/24. 4 dias para sair da penske cce sem transportadora</t>
+  </si>
+  <si>
+    <t>EXECUTIVA ENGENHARIA LTDA</t>
+  </si>
+  <si>
+    <t>Piranhas</t>
+  </si>
+  <si>
+    <t>18/06/2024 23:22:50</t>
+  </si>
+  <si>
+    <t>18/06/2024 08:18:20</t>
+  </si>
+  <si>
+    <t>Prev. Entrega 26/06</t>
+  </si>
+  <si>
+    <t>WALLACE ERICK DE MORAIS SOUZA</t>
+  </si>
+  <si>
+    <t>Limeira</t>
+  </si>
+  <si>
+    <t>EDUARDOGAZOTI (22)</t>
+  </si>
+  <si>
+    <t>BOOKED [Marcar Entrega]</t>
+  </si>
+  <si>
+    <t>24/06/2024 11:00:00</t>
+  </si>
+  <si>
+    <t>18/06/2024 08:18:21</t>
+  </si>
+  <si>
+    <t>Previsao de entrega: 01/07/24 - cte apenas do dia 26/06 com a transportadora</t>
+  </si>
+  <si>
+    <t>JOSE CARLOS RAMPELOTTI</t>
+  </si>
+  <si>
+    <t>Baixa Grande do Ribeiro</t>
+  </si>
+  <si>
+    <t>PI</t>
+  </si>
+  <si>
+    <t>18/06/2024 08:18:22</t>
+  </si>
+  <si>
+    <t>Prev. Entrega 25/06 - Prev. 28/06 atualizada</t>
+  </si>
+  <si>
+    <t>UNIAO COMERCIAL BARAO S/A LOCACAO E EMPR</t>
+  </si>
+  <si>
+    <t>Belo Horizonte</t>
+  </si>
+  <si>
+    <t>EM ENTREGA [Marcar Entrega]</t>
+  </si>
+  <si>
+    <t>24/06/2024</t>
+  </si>
+  <si>
+    <t>19/06/2024 07:46:18</t>
+  </si>
+  <si>
+    <t>WN COMERCIO E PRESTADORA DE SERVICOS EIR</t>
+  </si>
+  <si>
+    <t>00901673000112</t>
+  </si>
+  <si>
+    <t>São João Del Rei</t>
+  </si>
+  <si>
+    <t>MSOUZA (105)</t>
+  </si>
+  <si>
+    <t>CHEGADA NA CIDADE OU FILIAL DE DESTINO [Marcar Entrega]</t>
+  </si>
+  <si>
+    <t>24/06/2024 10:52:40</t>
+  </si>
+  <si>
+    <t>19/06/2024 07:46:19</t>
+  </si>
+  <si>
+    <t>TERRA FORTE SERVICOS DE TERRAPLENAGEM LT</t>
+  </si>
+  <si>
+    <t>Aparecida de Goiânia</t>
+  </si>
+  <si>
+    <t>COLIVEIRA (102)</t>
+  </si>
+  <si>
+    <t>23/06/2024</t>
+  </si>
+  <si>
+    <t>Km Transportes</t>
+  </si>
+  <si>
+    <t>19/06/2024 07:46:20</t>
+  </si>
+  <si>
+    <t>JOSIVAL NETO DE SOUZA</t>
+  </si>
+  <si>
+    <t>SAO FELIX DO XINGU</t>
+  </si>
+  <si>
+    <t>PREVISÃO DE ENTREGA [Marcar Entrega]</t>
+  </si>
+  <si>
+    <t>20/06/2024 08:17:54</t>
+  </si>
+  <si>
+    <t>INBESP-IND E B SUB-PROD ORi ANIMAL LTDA</t>
+  </si>
+  <si>
+    <t>06900555000176</t>
+  </si>
+  <si>
+    <t>Nossa Senhora do Livramento</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>JANIAMENDES (125)</t>
+  </si>
+  <si>
+    <t>MALOTE LIBERADO SEFAZ (45) [Marcar Entrega]</t>
+  </si>
+  <si>
+    <t>22/06/2024</t>
+  </si>
+  <si>
+    <t>Carvalina Transporte</t>
+  </si>
+  <si>
+    <t>20/06/2024 08:17:56</t>
+  </si>
+  <si>
+    <t>LYON COMERCIO DE PECAS PARA TRATORE A -</t>
+  </si>
+  <si>
+    <t>Novo Progresso</t>
+  </si>
+  <si>
+    <t>21/06/2024</t>
+  </si>
+  <si>
+    <t>20/06/2024 08:17:57</t>
+  </si>
+  <si>
+    <t>TOP STAR PECAS PARA TRATORES E MAQUINAS</t>
+  </si>
+  <si>
+    <t>08209554000105</t>
+  </si>
+  <si>
+    <t>Sinop</t>
+  </si>
+  <si>
+    <t>MULTPARTS COMERCIO DE PECAS LTDA</t>
+  </si>
+  <si>
+    <t>PONTES E LACERDA</t>
+  </si>
+  <si>
+    <t>SAIDA DE UNIDADE (15) [Marcar Entrega]</t>
+  </si>
+  <si>
+    <t>20/06/2024 08:17:58</t>
+  </si>
+  <si>
+    <t>Previsao de entrega: 28/06/24</t>
+  </si>
+  <si>
+    <t>WEBER TERRAPLENAGEM E LOCACAO DE MAQUINA</t>
+  </si>
+  <si>
+    <t>Blumenau</t>
+  </si>
+  <si>
+    <t>21/06/2024 08:33:00</t>
+  </si>
+  <si>
+    <t>DEXHEIMER E DASMACIEL TERRAPLENAGEM E TR</t>
+  </si>
+  <si>
+    <t>FONTOURA XAVIER</t>
+  </si>
+  <si>
+    <t>PRIMEIRA TENTATIVA DE ENTREGA (31) [Marcar Entrega]</t>
+  </si>
+  <si>
+    <t>21/06/2024 08:14:06</t>
+  </si>
+  <si>
+    <t>GUSTAVO RODRIGUES MARTINS</t>
+  </si>
+  <si>
+    <t>Rio Pomba</t>
+  </si>
+  <si>
+    <t>Prev. Entrega 28/06 - verificando</t>
+  </si>
+  <si>
+    <t>BELACCI DO BRASIL LTDA</t>
+  </si>
+  <si>
+    <t>Caçapava</t>
+  </si>
+  <si>
+    <t>KARENVEIGA (163)</t>
+  </si>
+  <si>
+    <t>21/06/2024 08:14:08</t>
+  </si>
+  <si>
+    <t>SMA MANUTENCAO DE EQUIPAMENTOS LTDA</t>
+  </si>
+  <si>
+    <t>CATAGUASES</t>
+  </si>
+  <si>
+    <t>21/06/2024 08:14:10</t>
+  </si>
+  <si>
+    <t>PREFEITURA DE CAMPOS NOVOS PAULISTA</t>
+  </si>
+  <si>
+    <t>CAMPOS NOVOS PAULISTA</t>
+  </si>
+  <si>
+    <t>JULIOPEDROZA (110)</t>
+  </si>
+  <si>
+    <t>27/06/2024 10:57:33</t>
+  </si>
+  <si>
+    <t>25/06/2024 10:25:39</t>
+  </si>
+  <si>
+    <t>Previsao de entrega: 02/07/24</t>
+  </si>
+  <si>
+    <t>CONSTRULAR MATERIAL DE CONSTRUCAO LTDA</t>
+  </si>
+  <si>
+    <t>04766715000291</t>
+  </si>
+  <si>
+    <t>Itanhaém</t>
+  </si>
+  <si>
+    <t>Prev. Entrega 01/07</t>
   </si>
 </sst>
 </file>
@@ -830,7 +1154,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0;\(#,##0\)"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -880,6 +1204,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -945,7 +1282,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -970,6 +1307,11 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -977,7 +1319,37 @@
     <cellStyle name="Normal 3" xfId="2" xr:uid="{C5C270AF-2E3A-4FBD-9257-6BC41C9504C2}"/>
     <cellStyle name="Normal 4" xfId="3" xr:uid="{2E9F3EA7-376B-4551-84C1-D324B6977A79}"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1239,11 +1611,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1328,91 +1700,91 @@
       </c>
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>231</v>
-      </c>
-      <c r="B2" s="9">
-        <v>26627354000235</v>
+      <c r="A2" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>264</v>
       </c>
       <c r="C2" s="9">
-        <v>144098</v>
+        <v>143758</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>228</v>
+        <v>254</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="16">
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>257</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>229</v>
+        <v>265</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>230</v>
+        <v>266</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>59</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
       <c r="K2" s="15">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="L2" s="9">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M2" s="9">
+        <v>7</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="9">
+        <v>143758</v>
+      </c>
+      <c r="P2" s="20" t="s">
+        <v>268</v>
+      </c>
+      <c r="Q2" s="10">
+        <v>45461</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="C3" s="9">
+        <v>143784</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="K3" s="15">
         <v>13</v>
-      </c>
-      <c r="N2" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="O2" s="9">
-        <v>144098</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="Q2" s="10">
-        <v>45469</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="B3" s="9">
-        <v>26627354000235</v>
-      </c>
-      <c r="C3" s="9">
-        <v>144112</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" s="16">
-        <v>0</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="K3" s="15">
-        <v>2</v>
       </c>
       <c r="L3" s="9">
         <v>5</v>
@@ -1421,77 +1793,1068 @@
         <v>13</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="O3" s="9">
-        <v>144112</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>227</v>
+        <v>143784</v>
+      </c>
+      <c r="P3" s="18" t="s">
+        <v>275</v>
       </c>
       <c r="Q3" s="10">
-        <v>45469</v>
+        <v>45468</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>231</v>
+        <v>276</v>
       </c>
       <c r="B4" s="9">
-        <v>26627354000235</v>
+        <v>43072799000134</v>
       </c>
       <c r="C4" s="9">
-        <v>144114</v>
+        <v>143915</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>228</v>
+        <v>277</v>
       </c>
       <c r="E4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="K4" s="15">
+        <v>9</v>
+      </c>
+      <c r="L4" s="9">
+        <v>2</v>
+      </c>
+      <c r="M4" s="9">
+        <v>8</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="O4" s="9">
+        <v>143915</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q4" s="8"/>
+    </row>
+    <row r="5" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>281</v>
+      </c>
+      <c r="B5" s="9">
+        <v>15184311000125</v>
+      </c>
+      <c r="C5" s="9">
+        <v>143919</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="K5" s="15">
+        <v>9</v>
+      </c>
+      <c r="L5" s="9">
+        <v>5</v>
+      </c>
+      <c r="M5" s="9">
+        <v>13</v>
+      </c>
+      <c r="N5" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5" s="9">
+        <v>143919</v>
+      </c>
+      <c r="P5" s="19" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q5" s="8"/>
+    </row>
+    <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="B6" s="9">
+        <v>49891068811</v>
+      </c>
+      <c r="C6" s="9">
+        <v>143929</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="K6" s="15">
+        <v>9</v>
+      </c>
+      <c r="L6" s="9">
+        <v>1</v>
+      </c>
+      <c r="M6" s="9">
+        <v>7</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="O6" s="9">
+        <v>143929</v>
+      </c>
+      <c r="P6" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="Q6" s="8"/>
+    </row>
+    <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="B7" s="9">
+        <v>27841324987</v>
+      </c>
+      <c r="C7" s="9">
+        <v>143936</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="K7" s="15">
+        <v>9</v>
+      </c>
+      <c r="L7" s="9">
+        <v>5</v>
+      </c>
+      <c r="M7" s="9">
+        <v>13</v>
+      </c>
+      <c r="N7" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="O7" s="21">
+        <v>143936</v>
+      </c>
+      <c r="P7" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="Q7" s="8"/>
+    </row>
+    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="B8" s="9">
+        <v>24013278000676</v>
+      </c>
+      <c r="C8" s="9">
+        <v>143963</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="16">
+        <v>0</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="K8" s="15">
+        <v>8</v>
+      </c>
+      <c r="L8" s="9">
+        <v>2</v>
+      </c>
+      <c r="M8" s="9">
+        <v>8</v>
+      </c>
+      <c r="N8" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="O8" s="9">
+        <v>143963</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q8" s="10">
+        <v>45469</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>303</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="C9" s="9">
+        <v>143975</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>306</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="K9" s="15">
+        <v>8</v>
+      </c>
+      <c r="L9" s="9">
+        <v>2</v>
+      </c>
+      <c r="M9" s="9">
+        <v>8</v>
+      </c>
+      <c r="N9" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="O9" s="21">
+        <v>143975</v>
+      </c>
+      <c r="P9" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q9" s="10">
+        <v>45469</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="B10" s="9">
+        <v>14838739000181</v>
+      </c>
+      <c r="C10" s="9">
+        <v>143976</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="K10" s="15">
+        <v>8</v>
+      </c>
+      <c r="L10" s="9">
+        <v>5</v>
+      </c>
+      <c r="M10" s="9">
+        <v>13</v>
+      </c>
+      <c r="N10" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="O10" s="9">
+        <v>143976</v>
+      </c>
+      <c r="P10" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q10" s="10">
+        <v>45469</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="B11" s="9">
+        <v>81884940544</v>
+      </c>
+      <c r="C11" s="9">
+        <v>144004</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="K11" s="15">
+        <v>7</v>
+      </c>
+      <c r="L11" s="9">
+        <v>5</v>
+      </c>
+      <c r="M11" s="9">
+        <v>13</v>
+      </c>
+      <c r="N11" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="O11" s="9">
+        <v>144004</v>
+      </c>
+      <c r="P11" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q11" s="10">
+        <v>45469</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="C12" s="9">
+        <v>144029</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="K12" s="15">
+        <v>7</v>
+      </c>
+      <c r="L12" s="9">
+        <v>6</v>
+      </c>
+      <c r="M12" s="9">
+        <v>11</v>
+      </c>
+      <c r="N12" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="O12" s="9">
+        <v>144029</v>
+      </c>
+      <c r="P12" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q12" s="10">
+        <v>45467</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="B13" s="9">
+        <v>18443349000163</v>
+      </c>
+      <c r="C13" s="9">
+        <v>144030</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F13" s="16">
+        <v>0</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>332</v>
+      </c>
+      <c r="K13" s="15">
+        <v>7</v>
+      </c>
+      <c r="L13" s="9">
+        <v>5</v>
+      </c>
+      <c r="M13" s="9">
+        <v>13</v>
+      </c>
+      <c r="N13" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="O13" s="9">
+        <v>144030</v>
+      </c>
+      <c r="P13" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q13" s="10">
+        <v>45469</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="C14" s="9">
+        <v>144031</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="F14" s="16">
+        <v>0</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>332</v>
+      </c>
+      <c r="K14" s="15">
+        <v>7</v>
+      </c>
+      <c r="L14" s="9">
+        <v>6</v>
+      </c>
+      <c r="M14" s="9">
+        <v>11</v>
+      </c>
+      <c r="N14" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="O14" s="9">
+        <v>144031</v>
+      </c>
+      <c r="P14" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q14" s="10">
+        <v>45467</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="B15" s="9">
+        <v>54027951000183</v>
+      </c>
+      <c r="C15" s="9">
+        <v>144034</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="F15" s="16">
+        <v>0</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="K15" s="15">
+        <v>7</v>
+      </c>
+      <c r="L15" s="9">
+        <v>6</v>
+      </c>
+      <c r="M15" s="9">
+        <v>11</v>
+      </c>
+      <c r="N15" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="O15" s="9">
+        <v>144034</v>
+      </c>
+      <c r="P15" s="11" t="s">
+        <v>340</v>
+      </c>
+      <c r="Q15" s="8"/>
+    </row>
+    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="C16" s="9">
+        <v>144044</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="F16" s="16">
+        <v>0</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="K16" s="15">
+        <v>7</v>
+      </c>
+      <c r="L16" s="9">
+        <v>6</v>
+      </c>
+      <c r="M16" s="9">
+        <v>11</v>
+      </c>
+      <c r="N16" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="O16" s="9">
+        <v>144044</v>
+      </c>
+      <c r="P16" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q16" s="10">
+        <v>45467</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="B17" s="9">
+        <v>10940568000146</v>
+      </c>
+      <c r="C17" s="9">
+        <v>144048</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="16">
-        <v>0</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="J4" s="8" t="s">
+      <c r="F17" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="G17" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="K4" s="15">
+      <c r="H17" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="K17" s="15">
+        <v>6</v>
+      </c>
+      <c r="L17" s="9">
+        <v>5</v>
+      </c>
+      <c r="M17" s="9">
+        <v>13</v>
+      </c>
+      <c r="N17" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="O17" s="9">
+        <v>144048</v>
+      </c>
+      <c r="P17" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q17" s="10">
+        <v>45468</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>344</v>
+      </c>
+      <c r="B18" s="9">
+        <v>29037679000175</v>
+      </c>
+      <c r="C18" s="9">
+        <v>144049</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>346</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="K18" s="15">
+        <v>6</v>
+      </c>
+      <c r="L18" s="9">
+        <v>5</v>
+      </c>
+      <c r="M18" s="9">
+        <v>13</v>
+      </c>
+      <c r="N18" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="O18" s="9">
+        <v>144049</v>
+      </c>
+      <c r="P18" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q18" s="10">
+        <v>45469</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="B19" s="9">
+        <v>36328293000188</v>
+      </c>
+      <c r="C19" s="9">
+        <v>144054</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="K19" s="15">
+        <v>6</v>
+      </c>
+      <c r="L19" s="9">
         <v>2</v>
       </c>
-      <c r="L4" s="9">
-        <v>5</v>
-      </c>
-      <c r="M4" s="9">
-        <v>13</v>
-      </c>
-      <c r="N4" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="O4" s="9">
-        <v>144114</v>
-      </c>
-      <c r="P4" s="8" t="s">
+      <c r="M19" s="9">
+        <v>8</v>
+      </c>
+      <c r="N19" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="O19" s="22">
+        <v>144054</v>
+      </c>
+      <c r="P19" s="18" t="s">
+        <v>350</v>
+      </c>
+      <c r="Q19" s="8"/>
+    </row>
+    <row r="20" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="B20" s="9">
+        <v>36445009000153</v>
+      </c>
+      <c r="C20" s="9">
+        <v>144076</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="K20" s="15">
+        <v>6</v>
+      </c>
+      <c r="L20" s="9">
+        <v>1</v>
+      </c>
+      <c r="M20" s="9">
+        <v>7</v>
+      </c>
+      <c r="N20" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="O20" s="9">
+        <v>144076</v>
+      </c>
+      <c r="P20" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="Q4" s="10">
+      <c r="Q20" s="10">
         <v>45469</v>
       </c>
+    </row>
+    <row r="21" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>355</v>
+      </c>
+      <c r="B21" s="9">
+        <v>37568100000129</v>
+      </c>
+      <c r="C21" s="9">
+        <v>144093</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>306</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="K21" s="15">
+        <v>6</v>
+      </c>
+      <c r="L21" s="9">
+        <v>2</v>
+      </c>
+      <c r="M21" s="9">
+        <v>8</v>
+      </c>
+      <c r="N21" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="O21" s="9">
+        <v>144093</v>
+      </c>
+      <c r="P21" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q21" s="10">
+        <v>45469</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="B22" s="9">
+        <v>46787644000172</v>
+      </c>
+      <c r="C22" s="9">
+        <v>144126</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>359</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>360</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="K22" s="15">
+        <v>2</v>
+      </c>
+      <c r="L22" s="9">
+        <v>1</v>
+      </c>
+      <c r="M22" s="9">
+        <v>7</v>
+      </c>
+      <c r="N22" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="O22" s="9">
+        <v>144126</v>
+      </c>
+      <c r="P22" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="Q22" s="8"/>
+    </row>
+    <row r="23" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>365</v>
+      </c>
+      <c r="C23" s="9">
+        <v>144147</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="K23" s="15">
+        <v>2</v>
+      </c>
+      <c r="L23" s="9">
+        <v>1</v>
+      </c>
+      <c r="M23" s="9">
+        <v>7</v>
+      </c>
+      <c r="N23" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="O23" s="9">
+        <v>144147</v>
+      </c>
+      <c r="P23" s="11" t="s">
+        <v>367</v>
+      </c>
+      <c r="Q23" s="8"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:S1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <customSheetViews>
     <customSheetView guid="{F4E47935-89ED-4945-9CD3-947E4497D6BA}" filter="1" showAutoFilter="1">
       <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-      <autoFilter ref="B1:P984" xr:uid="{B9A17C03-EB25-4BE9-A236-F0EEFCF55D1B}"/>
+      <autoFilter ref="B1:P984" xr:uid="{CBB9D2A2-DBA7-4751-B0FE-AA54DD2139C0}"/>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">
           <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="810247410"/>
@@ -1500,11 +2863,18 @@
     </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="O1">
-    <cfRule type="duplicateValues" dxfId="4" priority="714"/>
-    <cfRule type="duplicateValues" dxfId="3" priority="725"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="718"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="729"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C4">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+  <conditionalFormatting sqref="C6">
+    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C23">
+    <cfRule type="duplicateValues" dxfId="1" priority="746"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C6">
+    <cfRule type="duplicateValues" dxfId="0" priority="747"/>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -3716,10 +5086,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C7">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>